<commit_message>
script that automates running queries for all algos
</commit_message>
<xml_diff>
--- a/graph_expr/output/goodcol_outputs- Email_lb20_lb20_cyc_c_q7/Email_lb20_lb20_cyc_c_q7__simgrBYVIEWS_newcols_rmvEmpty.xlsx
+++ b/graph_expr/output/goodcol_outputs- Email_lb20_lb20_cyc_c_q7/Email_lb20_lb20_cyc_c_q7__simgrBYVIEWS_newcols_rmvEmpty.xlsx
@@ -218,13 +218,12 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -242,6 +241,13 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -254,6 +260,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -298,12 +310,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,19 +319,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -350,7 +366,7 @@
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.01953125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.03125" defaultRowHeight="13.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -774,7 +790,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.01171875" defaultRowHeight="17" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -888,40 +904,40 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="4" t="n">
-        <v>52709</v>
-      </c>
-      <c r="H4" s="4" t="n">
-        <v>91</v>
-      </c>
-      <c r="I4" s="4" t="n">
-        <v>22</v>
-      </c>
-      <c r="J4" s="4" t="n">
-        <v>214</v>
+      <c r="C4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>52709</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>74</v>
+      </c>
+      <c r="I4" s="6" t="n">
+        <v>22</v>
+      </c>
+      <c r="J4" s="6" t="n">
+        <v>183</v>
       </c>
       <c r="K4" s="5" t="n">
         <f aca="false">J4-H4</f>
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1102,7 +1118,7 @@
       <c r="F11" s="5" t="n">
         <v>0.13</v>
       </c>
-      <c r="G11" s="6" t="n">
+      <c r="G11" s="7" t="n">
         <v>52709</v>
       </c>
       <c r="H11" s="5" t="n">
@@ -1138,16 +1154,16 @@
       <c r="F12" s="5" t="n">
         <v>0.01</v>
       </c>
-      <c r="G12" s="6" t="n">
-        <v>52709</v>
-      </c>
-      <c r="H12" s="6" t="n">
+      <c r="G12" s="7" t="n">
+        <v>52709</v>
+      </c>
+      <c r="H12" s="7" t="n">
         <v>10246</v>
       </c>
       <c r="I12" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="J12" s="6" t="n">
+      <c r="J12" s="7" t="n">
         <v>11462</v>
       </c>
       <c r="K12" s="5" t="n">
@@ -1174,7 +1190,7 @@
       <c r="F13" s="5" t="n">
         <v>0.23</v>
       </c>
-      <c r="G13" s="6" t="n">
+      <c r="G13" s="7" t="n">
         <v>52709</v>
       </c>
       <c r="H13" s="5" t="n">

</xml_diff>